<commit_message>
Multi Chain Sampling with threading
</commit_message>
<xml_diff>
--- a/data/mossong/medlock_color.xlsx
+++ b/data/mossong/medlock_color.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dean\Dropbox\Dean\_Study\_Thesis\1Code\pertussis\data\mossong\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deanl\Dropbox\Dean\_Study\_Thesis\1code\pertussis_project\data\mossong\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,13 @@
   <sheets>
     <sheet name="medlock" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -876,10 +877,10 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="2">

</xml_diff>